<commit_message>
Selenium Season 3 programs till Apr 24th
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excels/Adactin Master Test Data.xlsx
+++ b/src/test/resources/testdata/excels/Adactin Master Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\009LiveTechWS\AutomationFramework\src\test\resources\testdata\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678D29B6-2690-4B42-BF0E-3EEF57D27193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D89492-F047-4F5C-B85D-993FD170622C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ECA7341F-7CE3-4EA7-B2BF-C9C26B540FCF}"/>
   </bookViews>
@@ -566,7 +566,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
@@ -712,7 +712,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>

</xml_diff>